<commit_message>
template udpated and session call added in re-registration upload
</commit_message>
<xml_diff>
--- a/public/webdata/ReRegistrationExcel.xlsx
+++ b/public/webdata/ReRegistrationExcel.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/B0208058/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/B0208058/Documents/slretailer-web-portal/public/webdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E6E012F-ED43-5E40-BBE8-545BE387212E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{460C3F93-8140-9B4E-8B23-C7F87CC02EF0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16160" xr2:uid="{AD25A3D4-5914-714C-9B57-13C12854785D}"/>
   </bookViews>
@@ -30,7 +30,7 @@
     <t>Customer MSISDN</t>
   </si>
   <si>
-    <t>Activation Date(dd-MM-yyyy HH:mm:ss)</t>
+    <t>Activation Date(dd/mm/yyyy)</t>
   </si>
 </sst>
 </file>
@@ -386,7 +386,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
CSV file updated and respected re-registration changes done
</commit_message>
<xml_diff>
--- a/public/webdata/ReRegistrationExcel.xlsx
+++ b/public/webdata/ReRegistrationExcel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/B0208058/Documents/slretailer-web-portal/public/webdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{460C3F93-8140-9B4E-8B23-C7F87CC02EF0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42D8D8B1-833D-1D4A-98AC-3743E487D626}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16160" xr2:uid="{AD25A3D4-5914-714C-9B57-13C12854785D}"/>
   </bookViews>
@@ -386,7 +386,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>